<commit_message>
i reviewed on task SRS_adminFeatures and mentioned the comments on the peering-review-sheet
</commit_message>
<xml_diff>
--- a/Project Management/PM_Peering_Review.xlsx
+++ b/Project Management/PM_Peering_Review.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maya Kind\Desktop\QA\Internal-Banking-System\Project Management\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A0530EC-E3AB-479F-A783-B1C71E8E7236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
@@ -18,13 +24,64 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>release version</t>
+  </si>
+  <si>
+    <t>task name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">task assigned to </t>
+  </si>
+  <si>
+    <t>Task Reviewed By</t>
+  </si>
+  <si>
+    <t>Comments</t>
+  </si>
+  <si>
+    <t>V1</t>
+  </si>
+  <si>
+    <t>SRS_adminFeatures</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Dina</t>
+  </si>
+  <si>
+    <t>Mayar</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clarify on (SRS_admin_editCst_02,SRS_admin_editAcc_05) what is the fields the admain which can the admin edit </t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -49,8 +106,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +399,71 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="G1:V2"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="14" max="14" width="10.77734375" customWidth="1"/>
+    <col min="15" max="15" width="17.21875" customWidth="1"/>
+    <col min="16" max="16" width="27" customWidth="1"/>
+    <col min="17" max="18" width="8.88671875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="2.109375" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="19.6640625" customWidth="1"/>
+    <col min="21" max="21" width="21.109375" customWidth="1"/>
+    <col min="22" max="22" width="23.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="7:22" ht="21" x14ac:dyDescent="0.4">
+      <c r="G1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3"/>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3"/>
+      <c r="N1" s="3"/>
+      <c r="O1" s="3"/>
+      <c r="P1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="7:22" x14ac:dyDescent="0.3">
+      <c r="O2" t="s">
+        <v>9</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="G1:O1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update REQ_SIQ file to contain customer responses
</commit_message>
<xml_diff>
--- a/Project Management/PM_Peering_Review.xlsx
+++ b/Project Management/PM_Peering_Review.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Quality Assurance\Internal-Banking-System\Project Management\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="ورقة1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
   <si>
     <t>release version</t>
   </si>
@@ -39,9 +34,6 @@
   </si>
   <si>
     <t>Comments</t>
-  </si>
-  <si>
-    <t>V1</t>
   </si>
   <si>
     <t>SRS_adminFeatures</t>
@@ -79,16 +71,34 @@
     <t xml:space="preserve">clarify on (SRS_admin_editCst_02,SRS_admin_editAcc_05) 
 what is the fields the admin which can the admin edit </t>
   </si>
+  <si>
+    <t>Aya</t>
+  </si>
+  <si>
+    <t>Sara</t>
+  </si>
+  <si>
+    <t>V3.0</t>
+  </si>
+  <si>
+    <t>SIQ_user_transactions_06
+SIQ_user_transactions_07
+SIQ_user_transactions_08
+theses SRS should be deleted as we can mention all the bank account details in SIQ_user_transactions_01</t>
+  </si>
+  <si>
+    <t>V1.0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -96,14 +106,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="14"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -145,10 +155,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -423,7 +433,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -431,102 +441,128 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="G1:V4"/>
+  <dimension ref="G1:V5"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="O5" sqref="O5"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="10" width="8.796875" style="1"/>
-    <col min="11" max="12" width="8.796875" style="1" customWidth="1"/>
-    <col min="13" max="13" width="6.8984375" style="1" customWidth="1"/>
-    <col min="14" max="14" width="10.796875" style="1" hidden="1" customWidth="1"/>
-    <col min="15" max="15" width="42.69921875" style="1" customWidth="1"/>
+    <col min="1" max="10" width="8.81640625" style="1"/>
+    <col min="11" max="12" width="8.81640625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="6.90625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="10.81640625" style="1" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="42.7265625" style="1" customWidth="1"/>
     <col min="16" max="16" width="27" style="1" customWidth="1"/>
-    <col min="17" max="18" width="8.8984375" style="1" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="2.09765625" style="1" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="19.69921875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="21.09765625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="23.09765625" style="1" customWidth="1"/>
-    <col min="23" max="16384" width="8.796875" style="1"/>
+    <col min="17" max="18" width="8.90625" style="1" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="2.08984375" style="1" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="19.7265625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="21.08984375" style="1" customWidth="1"/>
+    <col min="22" max="22" width="23.08984375" style="1" customWidth="1"/>
+    <col min="23" max="16384" width="8.81640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="7:22" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G1" s="3" t="s">
+    <row r="1" spans="7:22" ht="42.65" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="G1" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="3"/>
-      <c r="O1" s="3"/>
-      <c r="P1" s="4" t="s">
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="5"/>
-      <c r="R1" s="5"/>
-      <c r="S1" s="5"/>
-      <c r="T1" s="4" t="s">
+      <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
+      <c r="S1" s="4"/>
+      <c r="T1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="U1" s="4" t="s">
+      <c r="U1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="4" t="s">
+      <c r="V1" s="3" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="7:22" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="7:22" ht="54.65" customHeight="1" x14ac:dyDescent="0.35">
       <c r="O2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="T2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="U2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="7:22" ht="47.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="7:22" ht="99" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="O4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="7:22" ht="87" x14ac:dyDescent="0.35">
+      <c r="O5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="P5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="U2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="7:22" ht="47.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="P3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="U3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="7:22" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="O4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="T4" s="1" t="s">
+      <c r="Q5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="U4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>5</v>
+      <c r="S5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>